<commit_message>
Move dataset and models for recommender
</commit_message>
<xml_diff>
--- a/recommender.xlsx
+++ b/recommender.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\社交网络挖掘\POI\ours\snm-poi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{700B7D0E-04DF-4BED-88F2-ED979126E624}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{003472B7-C674-482E-9037-B33CD2F3285E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
   <si>
     <t>Key</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -92,6 +92,54 @@
   </si>
   <si>
     <t>Acc@20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>epoch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(20,)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EP20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LR0005</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LR0002</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(200,)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EP200</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gamma</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EP150</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(10,)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -99,8 +147,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="176" formatCode="0.000000_ "/>
+    <numFmt numFmtId="181" formatCode="0.000000_);[Red]\(0.000000\)"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -147,7 +196,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -156,6 +205,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -439,131 +491,392 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.75" customWidth="1"/>
-    <col min="3" max="3" width="9.08203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="9.08203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="10.75" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.75" customWidth="1"/>
+    <col min="7" max="7" width="9.08203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="9.08203125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="G1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="F2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2">
+      <c r="G2" s="4">
         <v>4.7601999999999998E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1000</v>
+      </c>
+      <c r="F3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1">
+      <c r="G3" s="4">
         <v>4.1952000000000003E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1000</v>
+      </c>
+      <c r="F4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="1">
+      <c r="G4" s="4">
         <v>0.133294</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1000</v>
+      </c>
+      <c r="F5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="1">
+      <c r="G5" s="4">
         <v>4.3194999999999997E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1000</v>
+      </c>
+      <c r="F6" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="1">
+      <c r="G6" s="4">
         <v>3.9694E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1000</v>
+      </c>
+      <c r="F7" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="1">
+      <c r="G7" s="4">
         <v>3.9040999999999999E-2</v>
       </c>
-      <c r="D7" s="2">
+      <c r="H7" s="2">
         <v>0.26666699999999999</v>
       </c>
-      <c r="E7" s="2">
+      <c r="I7" s="2">
         <v>0.33333299999999999</v>
       </c>
-      <c r="F7" s="2">
+      <c r="J7" s="2">
         <v>0.33333299999999999</v>
       </c>
-      <c r="G7" s="2">
+      <c r="K7" s="2">
         <v>0.4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2293</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="E9" s="1">
+        <v>200</v>
+      </c>
+      <c r="F9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="4">
+        <v>0.10539999999999999</v>
+      </c>
+      <c r="H9" s="2">
+        <v>3.7068999999999998E-2</v>
+      </c>
+      <c r="I9" s="2">
+        <v>8.9983999999999995E-2</v>
+      </c>
+      <c r="J9" s="2">
+        <v>0.12414600000000001</v>
+      </c>
+      <c r="K9" s="2">
+        <v>0.16528599999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="1">
+        <v>2293</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="E10" s="1">
+        <v>20</v>
+      </c>
+      <c r="F10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="4">
+        <v>0.141675</v>
+      </c>
+      <c r="H10" s="2">
+        <v>1.8026E-2</v>
+      </c>
+      <c r="I10" s="2">
+        <v>4.0557999999999997E-2</v>
+      </c>
+      <c r="J10" s="2">
+        <v>5.7276000000000001E-2</v>
+      </c>
+      <c r="K10" s="2">
+        <v>7.5010999999999994E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="1">
+        <v>2293</v>
+      </c>
+      <c r="C11" s="1">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="E11" s="1">
+        <v>20</v>
+      </c>
+      <c r="F11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="4">
+        <v>0.125113</v>
+      </c>
+      <c r="H11" s="2">
+        <v>2.3695000000000001E-2</v>
+      </c>
+      <c r="I11" s="2">
+        <v>6.0909999999999999E-2</v>
+      </c>
+      <c r="J11" s="2">
+        <v>8.1553E-2</v>
+      </c>
+      <c r="K11" s="2">
+        <v>0.106265</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="1">
+        <v>2293</v>
+      </c>
+      <c r="C12" s="1">
+        <v>2E-3</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="E12" s="1">
+        <v>20</v>
+      </c>
+      <c r="F12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="4">
+        <v>0.111472</v>
+      </c>
+      <c r="H12" s="2">
+        <v>3.1981000000000002E-2</v>
+      </c>
+      <c r="I12" s="2">
+        <v>7.6755000000000004E-2</v>
+      </c>
+      <c r="J12" s="2">
+        <v>0.10553899999999999</v>
+      </c>
+      <c r="K12" s="2">
+        <v>0.13824700000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="1">
+        <v>2293</v>
+      </c>
+      <c r="C13" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="E13" s="1">
+        <v>150</v>
+      </c>
+      <c r="F13" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13" s="4">
+        <v>0.101838</v>
+      </c>
+      <c r="H13" s="2">
+        <v>4.1867000000000001E-2</v>
+      </c>
+      <c r="I13" s="2">
+        <v>0.10364900000000001</v>
+      </c>
+      <c r="J13" s="2">
+        <v>0.13664799999999999</v>
+      </c>
+      <c r="K13" s="2">
+        <v>0.17866000000000001</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D1" r:id="rId1" xr:uid="{F5DE48D6-38AB-47BF-A257-6EB0B36EA5BE}"/>
-    <hyperlink ref="E1:G1" r:id="rId2" display="Acc@1" xr:uid="{6B237CCA-D0AA-42D7-804E-B7EB88E7E4C6}"/>
-    <hyperlink ref="E1" r:id="rId3" xr:uid="{C4985591-F8E1-4A1B-9210-C50ACFF7696E}"/>
-    <hyperlink ref="F1" r:id="rId4" xr:uid="{DFEB7D86-D8B2-4C2E-BFF4-8C954F59EABB}"/>
-    <hyperlink ref="G1" r:id="rId5" xr:uid="{A897BC3B-6A25-48DC-9A38-AA05DCBCC4B9}"/>
+    <hyperlink ref="H1" r:id="rId1" xr:uid="{F5DE48D6-38AB-47BF-A257-6EB0B36EA5BE}"/>
+    <hyperlink ref="I1:K1" r:id="rId2" display="Acc@1" xr:uid="{6B237CCA-D0AA-42D7-804E-B7EB88E7E4C6}"/>
+    <hyperlink ref="I1" r:id="rId3" xr:uid="{C4985591-F8E1-4A1B-9210-C50ACFF7696E}"/>
+    <hyperlink ref="J1" r:id="rId4" xr:uid="{DFEB7D86-D8B2-4C2E-BFF4-8C954F59EABB}"/>
+    <hyperlink ref="K1" r:id="rId5" xr:uid="{A897BC3B-6A25-48DC-9A38-AA05DCBCC4B9}"/>
+    <hyperlink ref="J11" r:id="rId6" display="Acc@10: 0.081553" xr:uid="{B3504AA9-9CBD-4F86-BF91-59762FD9E788}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update hyper-parameter for recommender
</commit_message>
<xml_diff>
--- a/recommender.xlsx
+++ b/recommender.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\社交网络挖掘\POI\ours\snm-poi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{003472B7-C674-482E-9037-B33CD2F3285E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10710B5E-EBB1-46BC-BB15-D8DA7C5B5F99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
   <si>
     <t>Key</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -140,6 +140,54 @@
   </si>
   <si>
     <t>(10,)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(20,40)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(10,20)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EP80</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EP250</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(10,20,30)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(10,20,30,40)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EP170</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EP225</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EP160</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(10,20,30,40,50)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EP400</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(20,40,60,80,100)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -149,7 +197,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="176" formatCode="0.000000_ "/>
-    <numFmt numFmtId="181" formatCode="0.000000_);[Red]\(0.000000\)"/>
+    <numFmt numFmtId="177" formatCode="0.000000_);[Red]\(0.000000\)"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -207,7 +255,7 @@
     <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -491,17 +539,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.75" bestFit="1" customWidth="1"/>
     <col min="2" max="5" width="10.75" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.75" customWidth="1"/>
+    <col min="6" max="6" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.08203125" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="11" width="9.08203125" style="2" bestFit="1" customWidth="1"/>
   </cols>
@@ -864,6 +912,216 @@
       </c>
       <c r="K13" s="2">
         <v>0.17866000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="1">
+        <v>2293</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="E14" s="1">
+        <v>250</v>
+      </c>
+      <c r="F14" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14" s="4">
+        <v>9.9975999999999995E-2</v>
+      </c>
+      <c r="H14" s="2">
+        <v>4.3610999999999997E-2</v>
+      </c>
+      <c r="I14" s="2">
+        <v>0.106992</v>
+      </c>
+      <c r="J14" s="2">
+        <v>0.14260800000000001</v>
+      </c>
+      <c r="K14" s="2">
+        <v>0.18243899999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="1">
+        <v>2293</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="E15" s="1">
+        <v>80</v>
+      </c>
+      <c r="F15" t="s">
+        <v>29</v>
+      </c>
+      <c r="G15" s="4">
+        <v>0.100019</v>
+      </c>
+      <c r="H15" s="2">
+        <v>4.3901999999999997E-2</v>
+      </c>
+      <c r="I15" s="2">
+        <v>0.10612000000000001</v>
+      </c>
+      <c r="J15" s="2">
+        <v>0.141154</v>
+      </c>
+      <c r="K15" s="2">
+        <v>0.18302099999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="1">
+        <v>2293</v>
+      </c>
+      <c r="C16" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="E16" s="1">
+        <v>170</v>
+      </c>
+      <c r="F16" t="s">
+        <v>33</v>
+      </c>
+      <c r="G16" s="4">
+        <v>9.9149000000000001E-2</v>
+      </c>
+      <c r="H16" s="2">
+        <v>4.521E-2</v>
+      </c>
+      <c r="I16" s="2">
+        <v>0.110481</v>
+      </c>
+      <c r="J16" s="2">
+        <v>0.14318900000000001</v>
+      </c>
+      <c r="K16" s="2">
+        <v>0.18985299999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="1">
+        <v>2293</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="E17" s="1">
+        <v>225</v>
+      </c>
+      <c r="F17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G17" s="4">
+        <v>9.8770999999999998E-2</v>
+      </c>
+      <c r="H17" s="2">
+        <v>4.521E-2</v>
+      </c>
+      <c r="I17" s="2">
+        <v>0.11019</v>
+      </c>
+      <c r="J17" s="2">
+        <v>0.14318900000000001</v>
+      </c>
+      <c r="K17" s="2">
+        <v>0.191888</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="1">
+        <v>2293</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="E18" s="1">
+        <v>160</v>
+      </c>
+      <c r="F18" t="s">
+        <v>38</v>
+      </c>
+      <c r="G18" s="4">
+        <v>9.8604999999999998E-2</v>
+      </c>
+      <c r="H18" s="2">
+        <v>4.5791999999999999E-2</v>
+      </c>
+      <c r="I18" s="2">
+        <v>0.110481</v>
+      </c>
+      <c r="J18" s="2">
+        <v>0.14391599999999999</v>
+      </c>
+      <c r="K18" s="2">
+        <v>0.19072500000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="1">
+        <v>2293</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="E19" s="1">
+        <v>400</v>
+      </c>
+      <c r="F19" t="s">
+        <v>40</v>
+      </c>
+      <c r="G19" s="4">
+        <v>9.8604999999999998E-2</v>
+      </c>
+      <c r="H19" s="2">
+        <v>4.4338000000000002E-2</v>
+      </c>
+      <c r="I19" s="2">
+        <v>0.10917300000000001</v>
+      </c>
+      <c r="J19" s="2">
+        <v>0.144207</v>
+      </c>
+      <c r="K19" s="2">
+        <v>0.19058</v>
       </c>
     </row>
   </sheetData>

</xml_diff>